<commit_message>
initial changes after feedback
</commit_message>
<xml_diff>
--- a/app/tables/adapt_missed_visit_form/forms/adapt_missed_visit_form/adapt_missed_visit_form.xlsx
+++ b/app/tables/adapt_missed_visit_form/forms/adapt_missed_visit_form/adapt_missed_visit_form.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="235">
   <si>
     <t>branch_label</t>
   </si>
@@ -112,12 +112,6 @@
     <t xml:space="preserve">Clinic name: </t>
   </si>
   <si>
-    <t>clinic_sub_country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clinic sub-country: </t>
-  </si>
-  <si>
     <t>end screen</t>
   </si>
   <si>
@@ -712,7 +706,22 @@
     <t>&lt;strong&gt;Section E: Reasons for Missed Visits(s) at Initial Clinic&lt;/strong&gt;</t>
   </si>
   <si>
+    <t>textarea</t>
+  </si>
+  <si>
     <t>selected(data('medical'), 'other_medical')</t>
+  </si>
+  <si>
+    <t>clinic_sub_county</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clinic sub-county: </t>
+  </si>
+  <si>
+    <t>Date.parse(data('date_first_return'))&gt; Date.parse(data('date_last_visit'))</t>
+  </si>
+  <si>
+    <t>Date.parse(data('date_last_visit')) &lt; new Date(new Date().setDate(new Date().getDate()-1))</t>
   </si>
 </sst>
 </file>
@@ -1110,8 +1119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G74" sqref="G74"/>
+    <sheetView tabSelected="1" topLeftCell="H7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,8 +1132,10 @@
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
     <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" style="8" customWidth="1"/>
     <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" customWidth="1"/>
+    <col min="19" max="19" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
@@ -1206,10 +1217,10 @@
         <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="135" x14ac:dyDescent="0.25">
@@ -1217,15 +1228,15 @@
         <v>23</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -1238,7 +1249,7 @@
         <v>23</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -1265,7 +1276,7 @@
     </row>
     <row r="10" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C10" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D10" s="13"/>
       <c r="J10" s="13"/>
@@ -1293,15 +1304,15 @@
         <v>24</v>
       </c>
       <c r="I13" t="s">
-        <v>31</v>
+        <v>231</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>32</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1316,160 +1327,166 @@
         <v>23</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="17" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="17" spans="3:19" ht="30" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="18" spans="3:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+      <c r="S17" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="18" spans="3:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D18" s="13"/>
       <c r="J18" s="13"/>
     </row>
-    <row r="19" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:19" ht="30" x14ac:dyDescent="0.25">
       <c r="G19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" t="s">
         <v>37</v>
       </c>
-      <c r="I19" t="s">
-        <v>39</v>
-      </c>
       <c r="J19" s="8" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+      <c r="S19" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="20" spans="3:19" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="21" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:19" ht="45" x14ac:dyDescent="0.25">
       <c r="G22" t="s">
         <v>23</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="23" spans="3:19" x14ac:dyDescent="0.25">
       <c r="G23" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" t="s">
         <v>41</v>
       </c>
-      <c r="H23" t="s">
-        <v>43</v>
-      </c>
       <c r="I23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="3:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="3:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D24" s="13"/>
       <c r="J24" s="13"/>
     </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:19" ht="30" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="3:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="3:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D26" s="13"/>
       <c r="J26" s="13"/>
     </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:19" x14ac:dyDescent="0.25">
       <c r="G27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I27" t="s">
+        <v>53</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="3:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>35</v>
+      </c>
+      <c r="I28" t="s">
+        <v>54</v>
+      </c>
+      <c r="J28" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="J27" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="G28" t="s">
-        <v>37</v>
-      </c>
-      <c r="I28" t="s">
-        <v>56</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="3:19" x14ac:dyDescent="0.25">
       <c r="G29" t="s">
         <v>24</v>
       </c>
       <c r="I29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="3:19" x14ac:dyDescent="0.25">
       <c r="G30" t="s">
         <v>24</v>
       </c>
       <c r="I30" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="3:19" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
         <v>24</v>
       </c>
       <c r="I31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="3:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="3:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C32" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D32" s="13"/>
       <c r="J32" s="13"/>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.25">
@@ -1482,29 +1499,29 @@
         <v>23</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="36" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G36" t="s">
+        <v>63</v>
+      </c>
+      <c r="H36" t="s">
+        <v>64</v>
+      </c>
+      <c r="I36" t="s">
         <v>65</v>
       </c>
-      <c r="H36" t="s">
-        <v>66</v>
-      </c>
-      <c r="I36" t="s">
-        <v>67</v>
-      </c>
       <c r="J36" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="3:10" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="C37" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J37" s="13"/>
     </row>
@@ -1514,32 +1531,32 @@
         <v>24</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="3:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C39" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D39" s="13"/>
       <c r="J39" s="13"/>
     </row>
     <row r="40" spans="3:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D40" s="13"/>
       <c r="J40" s="13"/>
     </row>
     <row r="41" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="3:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1551,13 +1568,13 @@
     </row>
     <row r="43" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I43" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J43" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="3:10" x14ac:dyDescent="0.25">
@@ -1565,10 +1582,10 @@
         <v>24</v>
       </c>
       <c r="I44" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J44" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="3:10" x14ac:dyDescent="0.25">
@@ -1576,22 +1593,22 @@
         <v>24</v>
       </c>
       <c r="I45" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J45" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="3:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D46" s="13"/>
       <c r="J46" s="13"/>
     </row>
     <row r="47" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="3:10" x14ac:dyDescent="0.25">
@@ -1601,24 +1618,24 @@
     </row>
     <row r="49" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G49" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H49" t="s">
+        <v>90</v>
+      </c>
+      <c r="I49" t="s">
+        <v>91</v>
+      </c>
+      <c r="J49" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="I49" t="s">
-        <v>93</v>
-      </c>
-      <c r="J49" s="8" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="50" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="3:10" x14ac:dyDescent="0.25">
@@ -1626,20 +1643,20 @@
         <v>24</v>
       </c>
       <c r="I51" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J51" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="3:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C53" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D53" s="8"/>
       <c r="J53" s="8"/>
@@ -1651,21 +1668,21 @@
     </row>
     <row r="55" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G55" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H55" t="s">
+        <v>107</v>
+      </c>
+      <c r="I55" t="s">
+        <v>108</v>
+      </c>
+      <c r="J55" s="8" t="s">
         <v>109</v>
-      </c>
-      <c r="I55" t="s">
-        <v>110</v>
-      </c>
-      <c r="J55" s="8" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="56" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="3:10" x14ac:dyDescent="0.25">
@@ -1675,24 +1692,24 @@
     </row>
     <row r="58" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G58" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H58" t="s">
+        <v>126</v>
+      </c>
+      <c r="I58" t="s">
+        <v>127</v>
+      </c>
+      <c r="J58" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="I58" t="s">
-        <v>129</v>
-      </c>
-      <c r="J58" s="8" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="59" spans="3:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="3:10" x14ac:dyDescent="0.25">
@@ -1700,143 +1717,146 @@
         <v>24</v>
       </c>
       <c r="I60" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J60" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="63" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G63" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H63" t="s">
+        <v>144</v>
+      </c>
+      <c r="I63" t="s">
+        <v>145</v>
+      </c>
+      <c r="J63" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="I63" t="s">
-        <v>147</v>
-      </c>
-      <c r="J63" s="8" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="64" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G64" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H64" t="s">
+        <v>149</v>
+      </c>
+      <c r="I64" t="s">
+        <v>148</v>
+      </c>
+      <c r="J64" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="65" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="G65" t="s">
+        <v>63</v>
+      </c>
+      <c r="H65" t="s">
+        <v>150</v>
+      </c>
+      <c r="I65" t="s">
+        <v>89</v>
+      </c>
+      <c r="J65" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="I64" t="s">
-        <v>150</v>
-      </c>
-      <c r="J64" s="8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="65" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="G65" t="s">
-        <v>65</v>
-      </c>
-      <c r="H65" t="s">
-        <v>152</v>
-      </c>
-      <c r="I65" t="s">
-        <v>91</v>
-      </c>
-      <c r="J65" s="8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="66" spans="3:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="67" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:17" ht="30" x14ac:dyDescent="0.25">
       <c r="G67" t="s">
         <v>23</v>
       </c>
       <c r="J67" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="68" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="G68" t="s">
+        <v>39</v>
+      </c>
+      <c r="H68" t="s">
+        <v>181</v>
+      </c>
+      <c r="I68" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="68" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="G68" t="s">
-        <v>41</v>
-      </c>
-      <c r="H68" t="s">
+      <c r="J68" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="I68" t="s">
+    </row>
+    <row r="69" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>66</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="70" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="G70" t="s">
         <v>184</v>
       </c>
-      <c r="J68" s="8" t="s">
+      <c r="I70" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="69" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
-        <v>68</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="70" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="G70" t="s">
+      <c r="J70" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="I70" t="s">
-        <v>187</v>
-      </c>
-      <c r="J70" s="8" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="71" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="Q70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="72" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73" spans="3:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G73" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="72" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C72" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="73" spans="3:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G73" t="s">
-        <v>65</v>
-      </c>
       <c r="H73" t="s">
+        <v>194</v>
+      </c>
+      <c r="I73" t="s">
+        <v>195</v>
+      </c>
+      <c r="J73" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="74" spans="3:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="G74" t="s">
+        <v>229</v>
+      </c>
+      <c r="I74" t="s">
         <v>196</v>
       </c>
-      <c r="I73" t="s">
+      <c r="J74" s="8" t="s">
         <v>197</v>
-      </c>
-      <c r="J73" s="8" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="74" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="G74" t="s">
-        <v>24</v>
-      </c>
-      <c r="I74" t="s">
-        <v>198</v>
-      </c>
-      <c r="J74" s="8" t="s">
-        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -1849,7 +1869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -1862,10 +1882,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>8</v>
@@ -1873,299 +1893,299 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B26" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B27" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B28" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C28" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B29" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C29" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B30" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C30" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B31" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C31" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B33" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2173,233 +2193,233 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B35" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C35" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B36" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C36" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B37" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C37" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B38" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C38" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B39" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C39" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B40" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C40" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B41" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C41" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B42" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C42" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B44" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C44" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B46" t="s">
+        <v>187</v>
+      </c>
+      <c r="C46" t="s">
         <v>189</v>
-      </c>
-      <c r="C46" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B47" t="s">
+        <v>188</v>
+      </c>
+      <c r="C47" t="s">
         <v>190</v>
-      </c>
-      <c r="C47" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B49" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C49" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B50" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C50" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B51" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C51" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B52" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C52" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B53" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C53" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B54" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C54" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B55" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C55" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B56" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C56" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B57" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C57" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B58" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C58" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2424,7 +2444,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>10</v>
@@ -2432,50 +2452,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
         <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2500,10 +2520,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>21</v>
@@ -2511,25 +2531,25 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B4" s="11">
         <v>20141008</v>
@@ -2538,11 +2558,11 @@
     </row>
     <row r="5" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>